<commit_message>
created and executed test cases for purchase page
</commit_message>
<xml_diff>
--- a/exec/symlex_vpn_windows/report_summary.xlsx
+++ b/exec/symlex_vpn_windows/report_summary.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\symlex_vpn_windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39FE6EF-59A7-4015-AD1C-8FB35B2BBBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26763C8B-120D-4F2D-BC16-9173B5FC189D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="2" r:id="rId1"/>
     <sheet name="free_bonus" sheetId="5" r:id="rId2"/>
-    <sheet name="redeem_voucher" sheetId="7" r:id="rId3"/>
-    <sheet name="logout" sheetId="6" r:id="rId4"/>
-    <sheet name="auto_connect" sheetId="4" r:id="rId5"/>
-    <sheet name="general(settings)" sheetId="3" r:id="rId6"/>
+    <sheet name="purchase_page" sheetId="8" r:id="rId3"/>
+    <sheet name="redeem_voucher" sheetId="7" r:id="rId4"/>
+    <sheet name="logout" sheetId="6" r:id="rId5"/>
+    <sheet name="auto_connect" sheetId="4" r:id="rId6"/>
+    <sheet name="general(settings)" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Features of enter vpn</t>
   </si>
@@ -122,6 +123,17 @@
   </si>
   <si>
     <t>SYMREDVOU-022</t>
+  </si>
+  <si>
+    <t>SYM-PP-04,
+SYM-PP-08,
+SYM-PP-019,
+SYM-PP-022,
+SYM-PP-024,
+SYM-PP-025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (15-02-24)</t>
   </si>
 </sst>
 </file>
@@ -744,10 +756,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20E9BD1-861C-4DAA-A578-3640159897E0}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="98.25" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D112B8-BA61-4323-A81E-60AEE54129B4}">
   <dimension ref="D2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -812,7 +893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A287E34E-8299-4D47-B00D-598C59273152}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -879,7 +960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -948,7 +1029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:G8"/>
   <sheetViews>

</xml_diff>

<commit_message>
created test cases for connection page and connected device page and created api_symlex_login_username & password
</commit_message>
<xml_diff>
--- a/exec/symlex_vpn_windows/report_summary.xlsx
+++ b/exec/symlex_vpn_windows/report_summary.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\symlex_vpn_windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5BC574-4F6E-4D24-B7C9-1551725A7BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE71BC00-B2F7-43F4-8F36-BABD197E784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="2" r:id="rId1"/>
     <sheet name="my_account" sheetId="10" r:id="rId2"/>
     <sheet name="protocols(setting)" sheetId="9" r:id="rId3"/>
-    <sheet name="ad_block_server" sheetId="12" r:id="rId4"/>
-    <sheet name="forget_password" sheetId="11" r:id="rId5"/>
-    <sheet name="free_bonus" sheetId="5" r:id="rId6"/>
-    <sheet name="purchase_page" sheetId="8" r:id="rId7"/>
-    <sheet name="redeem_voucher" sheetId="7" r:id="rId8"/>
-    <sheet name="logout" sheetId="6" r:id="rId9"/>
-    <sheet name="auto_connect" sheetId="4" r:id="rId10"/>
-    <sheet name="general(settings)" sheetId="3" r:id="rId11"/>
+    <sheet name="connection_page" sheetId="13" r:id="rId4"/>
+    <sheet name="ad_block_server" sheetId="12" r:id="rId5"/>
+    <sheet name="forget_password" sheetId="11" r:id="rId6"/>
+    <sheet name="free_bonus" sheetId="5" r:id="rId7"/>
+    <sheet name="purchase_page" sheetId="8" r:id="rId8"/>
+    <sheet name="redeem_voucher" sheetId="7" r:id="rId9"/>
+    <sheet name="connected_devices" sheetId="14" r:id="rId10"/>
+    <sheet name="logout" sheetId="6" r:id="rId11"/>
+    <sheet name="auto_connect" sheetId="4" r:id="rId12"/>
+    <sheet name="general(settings)" sheetId="3" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
   <si>
     <t>Features of enter vpn</t>
   </si>
@@ -105,10 +107,6 @@
   </si>
   <si>
     <t>Ref. ID of Failed Test Case</t>
-  </si>
-  <si>
-    <t>SYMFREEBON-074,
-SYMFREEBON-075</t>
   </si>
   <si>
     <t xml:space="preserve"> Test Case Summary (12-02-24)</t>
@@ -159,17 +157,37 @@
   <si>
     <t xml:space="preserve"> Test Case Summary (22-02-24)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (26-02-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_AC_011,
+TC_SYM_AC_012,
+TC_SYM_AC_013</t>
+  </si>
+  <si>
+    <t>SYMFREEBON-074,
+SYMFREEBON-075,
+SYMFREEBON-076</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -317,19 +335,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,21 +356,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,6 +762,140 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B3D4B-C81A-4118-8051-58CD51E77CE6}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="73.5" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A287E34E-8299-4D47-B00D-598C59273152}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="73.5" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -757,7 +912,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -798,7 +953,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:G8"/>
   <sheetViews>
@@ -825,7 +980,7 @@
   <sheetData>
     <row r="2" spans="3:7" ht="18.75">
       <c r="C2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="13"/>
     </row>
@@ -867,7 +1022,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +1051,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -937,7 +1092,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +1120,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -1006,7 +1161,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1018,10 +1173,79 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0240F835-33DB-4C28-A260-ECF0731AC899}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="98.25" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A33E54C-DEB5-4BB8-BB86-A2471A6B4B70}">
   <dimension ref="D2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1034,7 +1258,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -1084,7 +1308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0FE5E3-5A70-40FA-B724-E1A08306649D}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1101,7 +1325,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -1142,7 +1366,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1153,12 +1377,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D2:E8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1187,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="4:5" ht="18.75">
@@ -1195,7 +1419,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="18.75">
@@ -1210,8 +1434,8 @@
       <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>25</v>
+      <c r="E8" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1222,7 +1446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20E9BD1-861C-4DAA-A578-3640159897E0}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1239,7 +1463,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -1280,7 +1504,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1291,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D112B8-BA61-4323-A81E-60AEE54129B4}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1308,7 +1532,7 @@
   <sheetData>
     <row r="2" spans="4:5" ht="18.75">
       <c r="D2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="13"/>
     </row>
@@ -1349,75 +1573,8 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A287E34E-8299-4D47-B00D-598C59273152}">
-  <dimension ref="D2:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
-      <c r="D2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="4:5" ht="18.75">
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5" ht="18.75">
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" ht="18.75">
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" ht="18.75">
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" ht="73.5" customHeight="1">
-      <c r="D8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>